<commit_message>
chages to download pdf table data from customers index page
</commit_message>
<xml_diff>
--- a/Outputs/Customers.xlsx
+++ b/Outputs/Customers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="383">
   <si>
     <t>Company Name</t>
   </si>
@@ -1159,6 +1159,9 @@
   </si>
   <si>
     <t>Poland</t>
+  </si>
+  <si>
+    <t>Allen, Michael1212</t>
   </si>
   <si>
     <t>Evaluation Only. Created with Aspose.Cells for .NET.Copyright 2003 - 2018 Aspose Pty Ltd.</t>
@@ -1622,7 +1625,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
@@ -3476,6 +3479,26 @@
         <v>380</v>
       </c>
     </row>
+    <row r="93" spans="1:6" ht="12.75">
+      <c r="A93" t="s">
+        <v>36</v>
+      </c>
+      <c r="B93" t="s">
+        <v>381</v>
+      </c>
+      <c r="C93" t="s">
+        <v>38</v>
+      </c>
+      <c r="D93" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" t="s">
+        <v>10</v>
+      </c>
+      <c r="F93" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -3492,7 +3515,7 @@
   <sheetData>
     <row r="5" spans="1:1" ht="23.25" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>